<commit_message>
Changes in before method and after method. Creating test data added.
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15570" windowHeight="6330" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15570" windowHeight="6330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="VerifyLoginLogout" sheetId="1" r:id="rId1"/>
     <sheet name="emp" sheetId="2" r:id="rId2"/>
     <sheet name="AddUsers" sheetId="3" r:id="rId3"/>
+    <sheet name="InsertEmployees" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>UserName</t>
   </si>
@@ -79,12 +80,39 @@
   </si>
   <si>
     <t>user2</t>
+  </si>
+  <si>
+    <t>Emp_number</t>
+  </si>
+  <si>
+    <t>Emp_ID</t>
+  </si>
+  <si>
+    <t>Emp_Firstname</t>
+  </si>
+  <si>
+    <t>Emp_Lastname</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="\'\'"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,11 +165,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -591,4 +623,82 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>90</v>
+      </c>
+      <c r="B2" s="7">
+        <v>90</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>91</v>
+      </c>
+      <c r="B3" s="7">
+        <v>91</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>92</v>
+      </c>
+      <c r="B4" s="7">
+        <v>92</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>